<commit_message>
export_emperor 启动加载 .env；.gitignore 忽略 .env
</commit_message>
<xml_diff>
--- a/emperor_rank_export.xlsx
+++ b/emperor_rank_export.xlsx
@@ -629,8 +629,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>爱新觉罗
-玄烨</t>
+          <t>爱新觉罗玄烨</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1145,8 +1144,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>爱新觉罗
-弘历</t>
+          <t>爱新觉罗弘历</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1730,8 +1728,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>爱新觉罗
-皇太极</t>
+          <t>爱新觉罗皇太极</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1950,8 +1947,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>爱新觉罗
-胤禛</t>
+          <t>爱新觉罗胤禛</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2017,7 +2013,11 @@
           <t>西辽</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>辽德宗</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>耶律大石</t>
@@ -6189,8 +6189,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>爱新觉罗
-福临</t>
+          <t>爱新觉罗福临</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -6702,8 +6701,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>爱新觉罗
-努尔哈赤</t>
+          <t>爱新觉罗努尔哈赤</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -7361,8 +7359,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>爱新觉罗
-颙琰</t>
+          <t>爱新觉罗颙琰</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -8890,14 +8887,10 @@
       <c r="A116" t="n">
         <v>115</v>
       </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="B116" t="inlineStr"/>
       <c r="C116" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>西楚霸王</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -9340,8 +9333,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>爱新觉罗
-旻宁</t>
+          <t>爱新觉罗旻宁</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -11681,8 +11673,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>爱新觉罗
-奕詝</t>
+          <t>爱新觉罗奕詝</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -13289,8 +13280,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>爱新觉罗
-载湉</t>
+          <t>爱新觉罗载湉</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -15255,8 +15245,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>爱新觉罗
-载淳</t>
+          <t>爱新觉罗载淳</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
@@ -21626,8 +21615,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>爱新觉罗
-溥仪</t>
+          <t>爱新觉罗溥仪</t>
         </is>
       </c>
       <c r="E304" t="inlineStr"/>

</xml_diff>